<commit_message>
updated emissions targets with excel workbook for estimating shift away from forest land -> energy and adjusted target file
</commit_message>
<xml_diff>
--- a/ssp_modeling/output_postprocessing/data/emission_targets_uganda_inventory_aggregates.xlsx
+++ b/ssp_modeling/output_postprocessing/data/emission_targets_uganda_inventory_aggregates.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/git/ssp_uganda_data/ssp_modeling/output_postprocessing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ED7404D-8089-8148-BF35-BD211CA515B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD8F139-AD2F-574A-AC35-03452CA56723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="760" windowWidth="27240" windowHeight="19560" activeTab="1" xr2:uid="{E464A41F-DFF0-F54F-A542-A6E1A2B016CF}"/>
+    <workbookView xWindow="6240" yWindow="760" windowWidth="27240" windowHeight="19560" activeTab="3" xr2:uid="{E464A41F-DFF0-F54F-A542-A6E1A2B016CF}"/>
   </bookViews>
   <sheets>
     <sheet name="targets_raw_table2.8" sheetId="1" r:id="rId1"/>
     <sheet name="targets_allocated_table2.82" sheetId="2" r:id="rId2"/>
     <sheet name="allocation_worksheet" sheetId="3" r:id="rId3"/>
+    <sheet name="for_trajectory_modification" sheetId="4" r:id="rId4"/>
+    <sheet name="for_trajectory_modification_not" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="54">
   <si>
     <t>Subsector</t>
   </si>
@@ -170,6 +172,54 @@
   </si>
   <si>
     <t>NEW TABLE</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>forest_seq_mt_co2e</t>
+  </si>
+  <si>
+    <t>total_forestland_mt_co2e</t>
+  </si>
+  <si>
+    <t>total_removals_to_reallocate_mt_co2e</t>
+  </si>
+  <si>
+    <t>frac_allocation_inen</t>
+  </si>
+  <si>
+    <t>frac_allocation_scoe</t>
+  </si>
+  <si>
+    <t>total_conversions</t>
+  </si>
+  <si>
+    <t>firewood</t>
+  </si>
+  <si>
+    <t>scoe_commercial</t>
+  </si>
+  <si>
+    <t>scoe_residential</t>
+  </si>
+  <si>
+    <t>charcoal</t>
+  </si>
+  <si>
+    <t>scoe_total</t>
+  </si>
+  <si>
+    <t>inen_total</t>
+  </si>
+  <si>
+    <t>for years outside of 2015/2017, see table 2.19 for fractional allocation of wood emissions (using TJ) in INEN and 2.26 for use in SCOE</t>
+  </si>
+  <si>
+    <t>frac_inen</t>
+  </si>
+  <si>
+    <t>frac_scoe</t>
   </si>
 </sst>
 </file>
@@ -684,14 +734,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1070,7 +1123,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="A1:E12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1288,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDD48E8-375B-384F-88F2-CCDDDBC5EA0C}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1508,7 +1561,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T12" sqref="P1:T12"/>
+      <selection activeCell="L8" sqref="L8:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1536,7 +1589,7 @@
       <c r="H1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>37</v>
       </c>
       <c r="P1" t="s">
@@ -1577,7 +1630,7 @@
       <c r="I2">
         <v>2017</v>
       </c>
-      <c r="O2" s="3"/>
+      <c r="O2" s="4"/>
       <c r="P2" t="s">
         <v>26</v>
       </c>
@@ -1622,7 +1675,7 @@
       <c r="K3" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="3"/>
+      <c r="O3" s="4"/>
       <c r="P3" t="s">
         <v>2</v>
       </c>
@@ -1670,7 +1723,7 @@
       <c r="L4">
         <v>13581</v>
       </c>
-      <c r="O4" s="3"/>
+      <c r="O4" s="4"/>
       <c r="P4" t="s">
         <v>21</v>
       </c>
@@ -1720,7 +1773,7 @@
       <c r="L5">
         <v>1230</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O5" s="4"/>
       <c r="P5" t="s">
         <v>4</v>
       </c>
@@ -1755,7 +1808,7 @@
       <c r="E6">
         <v>1.0569999999999999</v>
       </c>
-      <c r="O6" s="3"/>
+      <c r="O6" s="4"/>
       <c r="P6" t="s">
         <v>6</v>
       </c>
@@ -1790,7 +1843,7 @@
       <c r="E7">
         <v>0.34970000000000001</v>
       </c>
-      <c r="O7" s="3"/>
+      <c r="O7" s="4"/>
       <c r="P7" t="s">
         <v>8</v>
       </c>
@@ -1830,7 +1883,7 @@
         <f>1-L9</f>
         <v>0.9094322951181798</v>
       </c>
-      <c r="O8" s="3"/>
+      <c r="O8" s="4"/>
       <c r="P8" t="s">
         <v>10</v>
       </c>
@@ -1870,7 +1923,7 @@
         <f>L5/L4</f>
         <v>9.0567704881820185E-2</v>
       </c>
-      <c r="O9" s="3"/>
+      <c r="O9" s="4"/>
       <c r="P9" t="s">
         <v>22</v>
       </c>
@@ -1903,7 +1956,7 @@
       <c r="E10">
         <v>3.3109999999999999</v>
       </c>
-      <c r="O10" s="3"/>
+      <c r="O10" s="4"/>
       <c r="P10" t="s">
         <v>12</v>
       </c>
@@ -1938,7 +1991,7 @@
       <c r="E11">
         <v>3.1680000000000001</v>
       </c>
-      <c r="O11" s="3"/>
+      <c r="O11" s="4"/>
       <c r="P11" t="s">
         <v>14</v>
       </c>
@@ -1971,7 +2024,7 @@
       <c r="E12">
         <v>7.0220000000000002</v>
       </c>
-      <c r="O12" s="3"/>
+      <c r="O12" s="4"/>
       <c r="P12" t="s">
         <v>24</v>
       </c>
@@ -1992,41 +2045,41 @@
       <c r="G13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O13" s="3"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f>$L$8*H5</f>
         <v>46.089317540534566</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <f>$L$8*I5</f>
         <v>49.424542256682123</v>
       </c>
-      <c r="O14" s="3"/>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f>$L$9*H5</f>
         <v>4.5899004594654293</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <f>$L$9*I5</f>
         <v>4.9220457433178701</v>
       </c>
-      <c r="O15" s="3"/>
+      <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="O16" s="3"/>
+      <c r="O16" s="4"/>
     </row>
     <row r="17" spans="15:15" x14ac:dyDescent="0.2">
-      <c r="O17" s="3"/>
+      <c r="O17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2034,4 +2087,464 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3408ABC3-66DC-A144-B535-1311BDA009EC}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1995</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B3" si="0">B3</f>
+        <v>-11.152403</v>
+      </c>
+      <c r="C2">
+        <v>1.617</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D6" si="1">C2-B2</f>
+        <v>12.769403000000001</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E5" si="2">10.611-0.155</f>
+        <v>10.456000000000001</v>
+      </c>
+      <c r="F2">
+        <v>6.1387806675792356E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.93861219332420764</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2000</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>-11.152403</v>
+      </c>
+      <c r="C3">
+        <v>6.2779999999999996</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>17.430402999999998</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="2"/>
+        <v>10.456000000000001</v>
+      </c>
+      <c r="F3">
+        <v>6.3512120769379607E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.93648787923062038</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2005</v>
+      </c>
+      <c r="B4">
+        <f>B5</f>
+        <v>-11.152403</v>
+      </c>
+      <c r="C4">
+        <v>16.245000000000001</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>27.397403000000001</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>10.456000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.1040455588053253</v>
+      </c>
+      <c r="G4">
+        <v>0.89595444119467471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2010</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(B6:B7)</f>
+        <v>-11.152403</v>
+      </c>
+      <c r="C5">
+        <v>30.027000000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>41.179403000000001</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>10.456000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.12321606503619273</v>
+      </c>
+      <c r="G5">
+        <v>0.87678393496380724</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2015</v>
+      </c>
+      <c r="B6">
+        <v>-11.023218</v>
+      </c>
+      <c r="C6">
+        <v>39.655999999999999</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>50.679217999999999</v>
+      </c>
+      <c r="E6">
+        <f>10.611-0.155</f>
+        <v>10.456000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.20038102681842607</v>
+      </c>
+      <c r="G6">
+        <v>0.79961897318157393</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2017</v>
+      </c>
+      <c r="B7">
+        <v>-11.281587999999999</v>
+      </c>
+      <c r="C7">
+        <v>43.064999999999998</v>
+      </c>
+      <c r="D7">
+        <f>C7-B7</f>
+        <v>54.346587999999997</v>
+      </c>
+      <c r="E7">
+        <f>10.611-0.392</f>
+        <v>10.219000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.15894039735099338</v>
+      </c>
+      <c r="G7">
+        <v>0.84105960264900659</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD336C9-742E-374D-BCFA-142FB31EAC4D}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1995</v>
+      </c>
+      <c r="D2">
+        <v>2000</v>
+      </c>
+      <c r="E2">
+        <v>2005</v>
+      </c>
+      <c r="F2">
+        <v>2010</v>
+      </c>
+      <c r="G2">
+        <v>2015</v>
+      </c>
+      <c r="H2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>2329</v>
+      </c>
+      <c r="D3">
+        <v>1683</v>
+      </c>
+      <c r="E3">
+        <v>6191</v>
+      </c>
+      <c r="F3">
+        <v>9490</v>
+      </c>
+      <c r="G3">
+        <v>9240</v>
+      </c>
+      <c r="H3">
+        <v>9240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>28664</v>
+      </c>
+      <c r="D4">
+        <v>38250</v>
+      </c>
+      <c r="E4">
+        <v>46210</v>
+      </c>
+      <c r="F4">
+        <v>55879</v>
+      </c>
+      <c r="G4">
+        <v>8207</v>
+      </c>
+      <c r="H4">
+        <v>7560</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>9333</v>
+      </c>
+      <c r="D5">
+        <v>14612</v>
+      </c>
+      <c r="E5">
+        <v>15778</v>
+      </c>
+      <c r="F5">
+        <v>1713</v>
+      </c>
+      <c r="G5">
+        <v>46200</v>
+      </c>
+      <c r="H5">
+        <v>46200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>164696</v>
+      </c>
+      <c r="D6">
+        <v>182614</v>
+      </c>
+      <c r="E6">
+        <v>227124</v>
+      </c>
+      <c r="F6">
+        <v>265533</v>
+      </c>
+      <c r="G6">
+        <v>345578</v>
+      </c>
+      <c r="H6">
+        <v>292600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C3:C6)</f>
+        <v>205022</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:H7" si="0">SUM(D3:D6)</f>
+        <v>237159</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>295303</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>332615</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>409225</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>355600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>13409</v>
+      </c>
+      <c r="D10">
+        <v>16084</v>
+      </c>
+      <c r="E10">
+        <v>34293</v>
+      </c>
+      <c r="F10">
+        <v>46743</v>
+      </c>
+      <c r="G10">
+        <v>102550</v>
+      </c>
+      <c r="H10">
+        <v>67200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <f>C10/(C10+C7)</f>
+        <v>6.1387806675792356E-2</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:H13" si="1">D10/(D10+D7)</f>
+        <v>6.3512120769379607E-2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.1040455588053253</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.12321606503619273</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.20038102681842607</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0.15894039735099338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14">
+        <f>1-C13</f>
+        <v>0.93861219332420764</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:H14" si="2">1-D13</f>
+        <v>0.93648787923062038</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>0.89595444119467471</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>0.87678393496380724</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>0.79961897318157393</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>0.84105960264900659</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>